<commit_message>
minor fixes, produce results
</commit_message>
<xml_diff>
--- a/output/output_2_labels.xlsx
+++ b/output/output_2_labels.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,11 +450,11 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Opinioni negative sul biglietto: troppo confusionario e poco intuitivo</t>
+          <t>Opinioni positive sul biglietto di gratta e vinci</t>
         </is>
       </c>
     </row>
@@ -463,219 +463,11 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Opinioni negative sulle caratteristiche visive del biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>14</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Opinioni contrastanti sul biglietto del gioco</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Opinioni negative sul costo elevato del biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Critiche specifiche al biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Risposte positive e soddisfatte sul biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Risposte che indicano l'apprezzamento generale del biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Opinioni sulla grafica del biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Opinioni positive sul biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>12</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Critiche specifiche al biglietto del gioco</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>10</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>Opinioni negative sul biglietto della lotteria</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>8</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Opinioni sul prezzo del biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Opinioni negative sulle probabilità di vincita del biglietto della lotteria</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Opinioni contrastanti sul gratta e vinci</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Opinioni sul biglietto: complessità e difficoltà di comprensione</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>11</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Opinioni negative sul biglietto della lotteria</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>16</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Opinioni positive sul biglietto</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>17</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Opinioni contrastanti sul gioco e suggerimenti per migliorarlo</t>
         </is>
       </c>
     </row>

</xml_diff>